<commit_message>
Latest push added ahpallstationpage and line appro select to text box
</commit_message>
<xml_diff>
--- a/templates/Excel/Line_Setup.xlsx
+++ b/templates/Excel/Line_Setup.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -621,69 +621,180 @@
           <t>OK</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
+      <c r="M2" t="n">
+        <v>20</v>
+      </c>
+      <c r="N2" t="n">
+        <v>30</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>32</v>
+      </c>
+      <c r="R2" t="n">
+        <v>32</v>
+      </c>
+      <c r="S2" t="n">
+        <v>22</v>
+      </c>
+      <c r="T2" t="n">
+        <v>22</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>All ok</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Suriya</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Prakash</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-01-29T18:57</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SHIFT_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>22</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>All ok</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test </t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>Suriya</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>Prakash</t>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>suriya</t>
         </is>
       </c>
     </row>

</xml_diff>